<commit_message>
implementation of dynamic ui + sharedmanager class
</commit_message>
<xml_diff>
--- a/projects.xlsx
+++ b/projects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Christensen\Desktop\finalprojectgit\CSC132Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Christensen\Desktop\finallocal\CSC132Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B83BBB-5F10-453B-9356-2EE2763D4D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC844D1B-A95C-4BF0-ADD7-B7E6ADA0E7AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="17115" windowHeight="10876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2753" yWindow="1230" windowWidth="12689" windowHeight="7733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
   <si>
     <t>name</t>
   </si>
@@ -56,6 +56,72 @@
   </si>
   <si>
     <t>George, Lucas, Disney</t>
+  </si>
+  <si>
+    <t>GOOBING</t>
+  </si>
+  <si>
+    <t>THE GOOBENING</t>
+  </si>
+  <si>
+    <t>GARRRR</t>
+  </si>
+  <si>
+    <t>I LOVE FISH</t>
+  </si>
+  <si>
+    <t>Salmon, Tuna, Mahi-Mahi</t>
+  </si>
+  <si>
+    <t>Goober, Goobin, Gob</t>
+  </si>
+  <si>
+    <t>AH, AHH, AHHH</t>
+  </si>
+  <si>
+    <t>GALIJTOHTOH</t>
+  </si>
+  <si>
+    <t>THE ONE PIECE IS REAL</t>
+  </si>
+  <si>
+    <t>LORUEM</t>
+  </si>
+  <si>
+    <t>jljkdasfljkfasjlkfdsajlfdas</t>
+  </si>
+  <si>
+    <t>jlfdasljadfs,fadshlj,afdslj</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>World</t>
+  </si>
+  <si>
+    <t>python,c#,c++</t>
+  </si>
+  <si>
+    <t>Comp Sci!!!</t>
+  </si>
+  <si>
+    <t>WOOOOOOHHHOOOOO</t>
+  </si>
+  <si>
+    <t>:),:3,xD</t>
+  </si>
+  <si>
+    <t>adfsfadsafds</t>
+  </si>
+  <si>
+    <t>fdsaafdsdasfdafsdfasdafs</t>
+  </si>
+  <si>
+    <t>dfffdfsf</t>
+  </si>
+  <si>
+    <t>location</t>
   </si>
 </sst>
 </file>
@@ -317,10 +383,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -328,7 +394,7 @@
     <col min="2" max="2" width="37.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -338,8 +404,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -349,8 +418,11 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -360,8 +432,11 @@
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -370,6 +445,289 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>